<commit_message>
Deployment to Lisa Win7. Fixes for Scheme Year 2015 xcom and log file SBI number
</commit_message>
<xml_diff>
--- a/Documents/Config/config_Win7.xlsx
+++ b/Documents/Config/config_Win7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5492044-3DA1-4E3C-B8A1-1084046592E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831CC881-BE0F-4CD2-953D-DFB381D47DD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -343,9 +343,6 @@
   </si>
   <si>
     <t>CPHLinkLookUp</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance 2020\2020 SBI_CPH Link\2020 SBI_CPH Link.xls</t>
   </si>
   <si>
     <t>folder path to cph link up sbi</t>
@@ -469,120 +466,164 @@
     <t>APHA Animal Welfare Inspection Instructions</t>
   </si>
   <si>
+    <t>CustomerUrlRegex</t>
+  </si>
+  <si>
+    <t>.*person\/(\d*)\/permissions</t>
+  </si>
+  <si>
+    <t>Regex to extract the customer number from the RP Url</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\In Progress\</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Ready To Be Receipted\</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Completed\</t>
+  </si>
+  <si>
+    <t>RPCustomerUrl</t>
+  </si>
+  <si>
+    <t>Url to navigate to the customer details page of the test version of RP</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/dashboard/</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>Inspections</t>
+  </si>
+  <si>
+    <t>CaseOrigin</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>SharepointURL</t>
+  </si>
+  <si>
+    <t>SharepointFilePath</t>
+  </si>
+  <si>
+    <t>Item URL for Legacy LookUp document on Sharepoint</t>
+  </si>
+  <si>
+    <t>https://defra.sharepoint.com/teams/Team1140</t>
+  </si>
+  <si>
+    <t>URL for Defra Sharepoint for legacy Look Up document</t>
+  </si>
+  <si>
+    <t>LegacyLookUpFilePath</t>
+  </si>
+  <si>
+    <t>File path to save Legacy Look up file to from Sharepoint</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\</t>
+  </si>
+  <si>
+    <t>LegacyLookUpSavePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rpa-csc-prod.crm4.dynamics.com/main.aspx                                                                </t>
+  </si>
+  <si>
+    <t>http://crosscompliancedatabase/intranet/xcompliance2015.nsf/</t>
+  </si>
+  <si>
+    <t>SM-RPA-XC SAG Reports</t>
+  </si>
+  <si>
+    <t>SM-RPA-XC Animal Health Stand alone and selected</t>
+  </si>
+  <si>
+    <t>SM-RPA-XCRPAreports</t>
+  </si>
+  <si>
+    <t>ExceptionsFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Exceptions</t>
+  </si>
+  <si>
+    <t>outlookExceptionsFolder</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\{0} SBI_CPH Link\2020 SBI_CPH Link.xls</t>
+  </si>
+  <si>
+    <t>/UserInstructions/XC%20Master%20List%20{0}%20v1.0.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\XC Master list {1} v1.0.xlsx</t>
+  </si>
+  <si>
+    <t>XCOM Info</t>
+  </si>
+  <si>
+    <t>XcomComment</t>
+  </si>
+  <si>
+    <t>Cross Compliance {1}{0}
+{2}
+{3}</t>
+  </si>
+  <si>
+    <t>The comment to be entered in to XCOM and the note in CRM. For compliant only.</t>
+  </si>
+  <si>
+    <t>SAGInspectionName</t>
+  </si>
+  <si>
+    <t>Sheep and Goats Inspection</t>
+  </si>
+  <si>
+    <t>Used in the XcomComment</t>
+  </si>
+  <si>
+    <t>RPAInspectionName</t>
+  </si>
+  <si>
+    <t>Rural Payments Agency Inspection</t>
+  </si>
+  <si>
+    <t>CIIInspectionName</t>
+  </si>
+  <si>
+    <t>Cattle Identification Inspection</t>
+  </si>
+  <si>
+    <t>AWInspectionName</t>
+  </si>
+  <si>
+    <t>Animal Welfare Inspection</t>
+  </si>
+  <si>
     <t>Team Leader Name:  Rob Mclean 
 {0}
-Inspection result: 2020 Cross Compliance {1} – {2}
+Inspection result: 2021 Cross Compliance {1} – {2}
 {0}
 {3}
 {0}
-Version of the 2020 Cross Compliance Processing – {4}: 
+Version of the 2021 Cross Compliance Processing – {4}: 
 {5}
 {0}
 Inspection result Letter/Email Sent: {6}
 {0}
 CRF and Supporting Documents added to CRM: {7}</t>
-  </si>
-  <si>
-    <t>CustomerUrlRegex</t>
-  </si>
-  <si>
-    <t>.*person\/(\d*)\/permissions</t>
-  </si>
-  <si>
-    <t>Regex to extract the customer number from the RP Url</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\In Progress\</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Ready To Be Receipted\</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Completed\</t>
-  </si>
-  <si>
-    <t>RPCustomerUrl</t>
-  </si>
-  <si>
-    <t>Url to navigate to the customer details page of the test version of RP</t>
-  </si>
-  <si>
-    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/dashboard/</t>
-  </si>
-  <si>
-    <t>CaseType</t>
-  </si>
-  <si>
-    <t>Inspections</t>
-  </si>
-  <si>
-    <t>CaseOrigin</t>
-  </si>
-  <si>
-    <t>Internal</t>
-  </si>
-  <si>
-    <t>SharepointURL</t>
-  </si>
-  <si>
-    <t>SharepointFilePath</t>
-  </si>
-  <si>
-    <t>/UserInstructions/XC%20Master%20List%202021%20v1.0.xlsx</t>
-  </si>
-  <si>
-    <t>Item URL for Legacy LookUp document on Sharepoint</t>
-  </si>
-  <si>
-    <t>https://defra.sharepoint.com/teams/Team1140</t>
-  </si>
-  <si>
-    <t>URL for Defra Sharepoint for legacy Look Up document</t>
-  </si>
-  <si>
-    <t>LegacyLookUpFilePath</t>
-  </si>
-  <si>
-    <t>File path to save Legacy Look up file to from Sharepoint</t>
-  </si>
-  <si>
-    <t>C:\Users\{0}\Desktop\</t>
-  </si>
-  <si>
-    <t>LegacyLookUpSavePath</t>
-  </si>
-  <si>
-    <t>C:\Users\{0}\Desktop\XC Master list 2021 v1.0.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://rpa-csc-prod.crm4.dynamics.com/main.aspx                                                                </t>
-  </si>
-  <si>
-    <t>http://crosscompliancedatabase/intranet/xcompliance2015.nsf/</t>
-  </si>
-  <si>
-    <t>SM-RPA-XC SAG Reports</t>
-  </si>
-  <si>
-    <t>SM-RPA-XC Animal Health Stand alone and selected</t>
-  </si>
-  <si>
-    <t>SM-RPA-XCRPAreports</t>
-  </si>
-  <si>
-    <t>ExceptionsFolder</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Exceptions</t>
-  </si>
-  <si>
-    <t>outlookExceptionsFolder</t>
-  </si>
-  <si>
-    <t>Exceptions</t>
   </si>
 </sst>
 </file>
@@ -712,8 +753,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C84" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C84" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C90" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C90" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -1020,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,10 +1095,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1239,7 +1280,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>31</v>
@@ -1283,7 +1324,7 @@
         <v>103</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>104</v>
@@ -1291,24 +1332,24 @@
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,7 +1375,7 @@
         <v>11</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
@@ -1444,81 +1485,81 @@
         <v>105</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1572,7 @@
         <v>65</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,7 +1580,7 @@
         <v>67</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1555,7 +1596,7 @@
         <v>66</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,146 +1609,146 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B70" s="4">
         <v>1</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B71" s="4">
         <v>1</v>
@@ -1715,7 +1756,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B72" s="4">
         <v>1</v>
@@ -1723,7 +1764,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B73" s="4">
         <v>1</v>
@@ -1731,7 +1772,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B74" s="4">
         <v>1</v>
@@ -1739,82 +1780,133 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>87</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>88</v>
+        <v>183</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>89</v>
+        <v>185</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>90</v>
+        <v>186</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>101</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>93</v>
+        <v>192</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>100</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>99</v>
+      <c r="A81" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>95</v>
+      <c r="A82" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+    <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cii date received change
</commit_message>
<xml_diff>
--- a/Documents/Config/config_Win7.xlsx
+++ b/Documents/Config/config_Win7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D027DE-2869-4C6C-A548-069261FC52D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B5DBC3-638C-4FD3-80EC-33E8A97A396D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="3555" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12435" yWindow="1515" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,9 +234,6 @@
     <t>CiiMailbox</t>
   </si>
   <si>
-    <t>CrossCompliance.DiscrepancyReports@rpa.gov.uk</t>
-  </si>
-  <si>
     <t>inProgressFolder</t>
   </si>
   <si>
@@ -624,6 +621,9 @@
   </si>
   <si>
     <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\{0} SBI_CPH Link\2020 SBI_CPH Link.xlsx</t>
+  </si>
+  <si>
+    <t>SM-RPA-Cross Compliance CII Discrepancy Reports</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,95 +1095,95 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>31</v>
@@ -1321,35 +1321,35 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>11</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
@@ -1482,84 +1482,84 @@
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>65</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1580,7 +1580,7 @@
         <v>67</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>68</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>69</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,159 +1596,159 @@
         <v>66</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B70" s="4">
         <v>1</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="4">
         <v>1</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="4">
         <v>1</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B73" s="4">
         <v>1</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B74" s="4">
         <v>1</v>
@@ -1780,53 +1780,53 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1836,77 +1836,77 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>